<commit_message>
this version has Post and get methods
</commit_message>
<xml_diff>
--- a/RestAssured/config/file.xlsx
+++ b/RestAssured/config/file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">url</t>
   </si>
@@ -41,6 +41,14 @@
   </si>
   <si>
     <t xml:space="preserve">harry234@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "template": "Your otac {OTAC}",
+  "subject": "test",
+  "address": "idtest@mailinator.com",
+  "senderAddress": "idtest@mailinator.com"
+}</t>
   </si>
   <si>
     <t xml:space="preserve">harry23@mailinator.com</t>
@@ -117,9 +125,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -139,10 +151,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -168,7 +180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -177,6 +189,9 @@
       </c>
       <c r="E2" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -187,7 +202,7 @@
         <v>448147724431</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
this version has both ref and QA env
</commit_message>
<xml_diff>
--- a/RestAssured/config/file.xlsx
+++ b/RestAssured/config/file.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">url</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Email-id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Json Body</t>
   </si>
   <si>
     <t xml:space="preserve">identity/v1/identity/EMAIL/{email}/details</t>
@@ -66,6 +69,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,13 +158,15 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="66.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -179,30 +185,33 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>448147724401</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>448147724431</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>